<commit_message>
edited some pinar stuff
</commit_message>
<xml_diff>
--- a/output/gpx_191010_pinar.xlsx
+++ b/output/gpx_191010_pinar.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elahi/github/coding/output/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AA1271-E8DC-4343-B3E7-48B9FDBBF458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="4720" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8780" yWindow="2960" windowWidth="32040" windowHeight="14420"/>
   </bookViews>
   <sheets>
     <sheet name="gpx_191010_pinar" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>lon</t>
   </si>
@@ -94,9 +93,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>I thought I got the waypoint for the northeast corner of the property but I didn't</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jog on eastern fence. </t>
   </si>
   <si>
@@ -140,12 +136,15 @@
   </si>
   <si>
     <t>Hypothesized limit of southern boundary along fence (measured 67.8 ft from jog on eastern fence)</t>
+  </si>
+  <si>
+    <t>I thought I got the waypoint for the northeast corner of the property but I didn't; these values are from google maps (I checked point 15 and it was correct to the 4th decimal)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -727,7 +726,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -779,7 +778,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -973,21 +972,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
@@ -996,7 +995,7 @@
     <col min="7" max="7" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1019,12 +1018,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>-121.906856</v>
+      </c>
+      <c r="B2">
+        <v>36.593389999999999</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -1039,10 +1038,10 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>-121.907055</v>
       </c>
@@ -1062,10 +1061,10 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>-121.907032</v>
       </c>
@@ -1085,10 +1084,10 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>-121.907178</v>
       </c>
@@ -1108,10 +1107,10 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>-121.907141</v>
       </c>
@@ -1131,10 +1130,10 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>-121.90723300000001</v>
       </c>
@@ -1154,10 +1153,10 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>-121.90724400000001</v>
       </c>
@@ -1177,10 +1176,10 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>-121.90725399999999</v>
       </c>
@@ -1200,10 +1199,10 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>-121.907155</v>
       </c>
@@ -1223,10 +1222,10 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>-121.907043</v>
       </c>
@@ -1246,10 +1245,10 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>-121.906919</v>
       </c>
@@ -1269,10 +1268,10 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>-121.90697900000001</v>
       </c>
@@ -1292,10 +1291,10 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>-121.906925</v>
       </c>
@@ -1315,10 +1314,10 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>-121.906888</v>
       </c>
@@ -1338,10 +1337,10 @@
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>-121.90690600000001</v>
       </c>
@@ -1361,10 +1360,10 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>-121.907037</v>
       </c>
@@ -1384,10 +1383,15 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>